<commit_message>
A hell of a mess
</commit_message>
<xml_diff>
--- a/tests/testthat/comment-on-blank-cell.xlsx
+++ b/tests/testthat/comment-on-blank-cell.xlsx
@@ -19,7 +19,7 @@
     <author>nacnudus</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -384,9 +384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -399,8 +401,10 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>